<commit_message>
Formato de Informe de proyecto
</commit_message>
<xml_diff>
--- a/Asistencia.xlsx
+++ b/Asistencia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\JAVA\JDBC\JDBC_2020_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A95E01-A195-404F-ABA1-69440F1E91C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ED88C6-7FD6-4366-8796-FB944F2ABDD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>NRO</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>04.OCT.20</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +903,9 @@
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
@@ -959,8 +964,9 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A4:F4"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>